<commit_message>
Diagram Modificate and Aggregate PDF
Diagram Modificate and Aggregate PDF
</commit_message>
<xml_diff>
--- a/04-TEST/PRUEBAS UNITARIAS/PLANTILLA_PRUEBAS_DE_SOFTWARE/Plantilla_Pruebas_de_Software_S.O.E.xlsx
+++ b/04-TEST/PRUEBAS UNITARIAS/PLANTILLA_PRUEBAS_DE_SOFTWARE/Plantilla_Pruebas_de_Software_S.O.E.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c7f5dae58cac8d6/Documentos/SOE/04-TEST/PRUEBAS UNITARIAS/PLANTILLA_PRUEBAS_DE_SOFTWARE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{D28DF50D-15A6-46AF-9D54-C878F891D79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54C0D5D5-77B6-4F7B-A77D-E7C89B885F52}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{D28DF50D-15A6-46AF-9D54-C878F891D79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6351C99-1476-4283-8324-26225D8B0E14}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inicio Sesión" sheetId="1" r:id="rId1"/>
@@ -646,9 +646,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -688,48 +685,51 @@
     <xf numFmtId="0" fontId="13" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="14" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="14" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1247,8 +1247,8 @@
   </sheetPr>
   <dimension ref="B2:J24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1274,14 +1274,14 @@
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="2:10" ht="15.6">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="26"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="2:10" ht="27.75" customHeight="1">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="24" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1290,16 +1290,16 @@
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="2:10" ht="60">
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="27" t="s">
         <v>94</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="2:10" ht="28.5" customHeight="1">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="24" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="6">
@@ -1308,7 +1308,7 @@
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="2:10" ht="26.25" customHeight="1">
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="24" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="6">
@@ -1316,15 +1316,15 @@
       </c>
     </row>
     <row r="10" spans="2:10" ht="28.5" customHeight="1">
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="26" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="30" customHeight="1">
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="25" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1332,16 +1332,16 @@
       </c>
     </row>
     <row r="12" spans="2:10" ht="46.8" customHeight="1">
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="27" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="13.2"/>
     <row r="16" spans="2:10" ht="73.5" customHeight="1">
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="28" t="s">
         <v>92</v>
       </c>
       <c r="C16" s="7" t="s">
@@ -1359,7 +1359,7 @@
       <c r="G16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H16" s="39" t="s">
         <v>17</v>
       </c>
       <c r="I16" s="8" t="s">
@@ -1370,135 +1370,135 @@
       </c>
     </row>
     <row r="17" spans="2:10" ht="102" customHeight="1">
-      <c r="B17" s="32">
+      <c r="B17" s="29">
         <v>1</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="I17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="12">
+      <c r="J17" s="11">
         <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="100.2" customHeight="1">
-      <c r="B18" s="32">
+      <c r="B18" s="29">
         <v>2</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H18" s="13" t="s">
+      <c r="H18" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="I18" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="12">
+      <c r="J18" s="11">
         <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="99" customHeight="1">
-      <c r="B19" s="32">
+      <c r="B19" s="29">
         <v>3</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="12">
+      <c r="J19" s="11">
         <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="99" customHeight="1">
-      <c r="B20" s="32">
+      <c r="B20" s="29">
         <v>4</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="C20" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I20" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="12">
+      <c r="J20" s="11">
         <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="13.2">
-      <c r="D21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="D21" s="13"/>
+      <c r="F21" s="13"/>
     </row>
     <row r="22" spans="2:10" ht="15">
-      <c r="D22" s="15"/>
-      <c r="F22" s="15"/>
+      <c r="D22" s="14"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:10" ht="15">
-      <c r="D23" s="15"/>
-      <c r="F23" s="16"/>
+      <c r="D23" s="14"/>
+      <c r="F23" s="15"/>
     </row>
     <row r="24" spans="2:10" ht="15">
-      <c r="F24" s="16"/>
+      <c r="F24" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1542,14 +1542,14 @@
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="2:10" ht="15.6">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="26"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="2:10" ht="27.75" customHeight="1">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="24" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1558,16 +1558,16 @@
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="2:10" ht="60">
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="27" t="s">
         <v>94</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="2:10" ht="28.5" customHeight="1">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="24" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="6">
@@ -1576,7 +1576,7 @@
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="2:10" ht="26.25" customHeight="1">
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="24" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="6">
@@ -1584,37 +1584,37 @@
       </c>
     </row>
     <row r="10" spans="2:10" ht="28.5" customHeight="1">
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
     </row>
     <row r="11" spans="2:10" ht="30" customHeight="1">
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="27" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="42.6" customHeight="1">
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="27" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="61.2" customHeight="1"/>
     <row r="16" spans="2:10" ht="82.8" customHeight="1">
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="31" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="7" t="s">
@@ -1640,135 +1640,135 @@
       </c>
     </row>
     <row r="17" spans="2:10" ht="100.2" customHeight="1">
-      <c r="B17" s="32">
+      <c r="B17" s="29">
         <v>5</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="I17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="12">
+      <c r="J17" s="11">
         <v>0.5</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="100.2" customHeight="1">
-      <c r="B18" s="32">
+      <c r="B18" s="29">
         <v>6</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="I18" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="12">
+      <c r="J18" s="11">
         <v>0.50347222222222221</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="100.8" customHeight="1">
-      <c r="B19" s="32">
+      <c r="B19" s="29">
         <v>7</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="12">
+      <c r="J19" s="11">
         <v>0.50347222222222221</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="100.8" customHeight="1">
-      <c r="B20" s="32">
+      <c r="B20" s="29">
         <v>8</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I20" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="12">
+      <c r="J20" s="11">
         <v>0.50347222222222221</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="13.2">
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
     </row>
     <row r="22" spans="2:10" ht="15">
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
     </row>
     <row r="23" spans="2:10" ht="15">
-      <c r="D23" s="15"/>
-      <c r="E23" s="16"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="15"/>
     </row>
     <row r="24" spans="2:10" ht="15">
-      <c r="E24" s="16"/>
+      <c r="E24" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1786,7 +1786,7 @@
   </sheetPr>
   <dimension ref="B2:J24"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1813,14 +1813,14 @@
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="26"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="2:10" ht="27.75" customHeight="1">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="24" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1829,16 +1829,16 @@
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="2:10" ht="60">
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="27" t="s">
         <v>94</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="2:10" ht="28.5" customHeight="1">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="24" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="6">
@@ -1847,7 +1847,7 @@
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="2:10" ht="26.25" customHeight="1">
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="24" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="6">
@@ -1855,35 +1855,35 @@
       </c>
     </row>
     <row r="10" spans="2:10" ht="28.5" customHeight="1">
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="26" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="30" customHeight="1">
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="27" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="54" customHeight="1">
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="27" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="13.2"/>
     <row r="16" spans="2:10" ht="99.6" customHeight="1">
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="31" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="7" t="s">
@@ -1909,135 +1909,135 @@
       </c>
     </row>
     <row r="17" spans="2:10" ht="100.2" customHeight="1">
-      <c r="B17" s="32">
+      <c r="B17" s="29">
         <v>9</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="I17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="12">
+      <c r="J17" s="11">
         <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="100.2" customHeight="1">
-      <c r="B18" s="32">
+      <c r="B18" s="29">
         <v>10</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="I18" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="12">
+      <c r="J18" s="11">
         <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="99" customHeight="1">
-      <c r="B19" s="32">
+      <c r="B19" s="29">
         <v>11</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="12">
+      <c r="J19" s="11">
         <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="115.8" customHeight="1">
-      <c r="B20" s="32">
+      <c r="B20" s="29">
         <v>12</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I20" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="12">
+      <c r="J20" s="11">
         <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="13.2">
-      <c r="D21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="D21" s="13"/>
+      <c r="F21" s="13"/>
     </row>
     <row r="22" spans="2:10" ht="15">
-      <c r="D22" s="15"/>
-      <c r="F22" s="15"/>
+      <c r="D22" s="14"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:10" ht="15">
-      <c r="D23" s="15"/>
-      <c r="F23" s="16"/>
+      <c r="D23" s="14"/>
+      <c r="F23" s="15"/>
     </row>
     <row r="24" spans="2:10" ht="15">
-      <c r="F24" s="16"/>
+      <c r="F24" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2082,14 +2082,14 @@
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="26"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="2:10" ht="27.75" customHeight="1">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="24" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -2098,16 +2098,16 @@
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="2:10" ht="60">
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="27" t="s">
         <v>94</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="2:10" ht="28.5" customHeight="1">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="24" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="6">
@@ -2116,7 +2116,7 @@
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="2:10" ht="26.25" customHeight="1">
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="24" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="6">
@@ -2124,189 +2124,189 @@
       </c>
     </row>
     <row r="10" spans="2:10" ht="28.5" customHeight="1">
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="26" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="30" customHeight="1">
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="27" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="52.8" customHeight="1">
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="27" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="13.2"/>
     <row r="16" spans="2:10" ht="81" customHeight="1">
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="37" t="s">
+      <c r="E16" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="37" t="s">
+      <c r="F16" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="37" t="s">
+      <c r="G16" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="37" t="s">
+      <c r="H16" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="37" t="s">
+      <c r="I16" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="J16" s="37" t="s">
+      <c r="J16" s="34" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="99.6" customHeight="1">
-      <c r="B17" s="32">
+      <c r="B17" s="29">
         <v>13</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="I17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="12">
+      <c r="J17" s="11">
         <v>0.625</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="100.8" customHeight="1">
-      <c r="B18" s="32">
+      <c r="B18" s="29">
         <v>14</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="I18" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="12">
+      <c r="J18" s="11">
         <v>0.625</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="99.6" customHeight="1">
-      <c r="B19" s="32">
+      <c r="B19" s="29">
         <v>15</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="12">
+      <c r="J19" s="11">
         <v>0.625</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="100.8" customHeight="1">
-      <c r="B20" s="32">
+      <c r="B20" s="29">
         <v>16</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I20" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="12">
+      <c r="J20" s="11">
         <v>0.625</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="13.2">
-      <c r="D21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="D21" s="13"/>
+      <c r="F21" s="13"/>
     </row>
     <row r="22" spans="2:10" ht="15">
-      <c r="D22" s="15"/>
-      <c r="F22" s="15"/>
+      <c r="D22" s="14"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:10" ht="15">
-      <c r="D23" s="15"/>
-      <c r="F23" s="16"/>
+      <c r="D23" s="14"/>
+      <c r="F23" s="15"/>
     </row>
     <row r="24" spans="2:10" ht="15">
-      <c r="F24" s="16"/>
+      <c r="F24" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2324,7 +2324,7 @@
   </sheetPr>
   <dimension ref="B2:J24"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -2351,14 +2351,14 @@
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="2:10" ht="26.4" customHeight="1">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="26"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="2:10" ht="27.75" customHeight="1">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="24" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -2367,16 +2367,16 @@
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="2:10" ht="60">
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="27" t="s">
         <v>94</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="2:10" ht="28.5" customHeight="1">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="24" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="6">
@@ -2385,7 +2385,7 @@
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="2:10" ht="26.25" customHeight="1">
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="24" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="6">
@@ -2393,189 +2393,189 @@
       </c>
     </row>
     <row r="10" spans="2:10" ht="28.5" customHeight="1">
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="26" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="30" customHeight="1">
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="27" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="63" customHeight="1">
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="27" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="13.2"/>
     <row r="16" spans="2:10" ht="60" customHeight="1">
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="37" t="s">
+      <c r="E16" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="37" t="s">
+      <c r="F16" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="37" t="s">
+      <c r="G16" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="37" t="s">
+      <c r="H16" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="37" t="s">
+      <c r="I16" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="J16" s="37" t="s">
+      <c r="J16" s="34" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="99.6" customHeight="1">
-      <c r="B17" s="32">
+      <c r="B17" s="29">
         <v>17</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="I17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="12">
+      <c r="J17" s="11">
         <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="99" customHeight="1">
-      <c r="B18" s="32">
+      <c r="B18" s="29">
         <v>18</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="I18" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="12">
+      <c r="J18" s="11">
         <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="99.6" customHeight="1">
-      <c r="B19" s="32">
+      <c r="B19" s="29">
         <v>19</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="12">
+      <c r="J19" s="11">
         <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="100.2" customHeight="1">
-      <c r="B20" s="32">
+      <c r="B20" s="29">
         <v>20</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I20" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="12">
+      <c r="J20" s="11">
         <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="13.2">
-      <c r="D21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="D21" s="13"/>
+      <c r="F21" s="13"/>
     </row>
     <row r="22" spans="2:10" ht="15">
-      <c r="D22" s="15"/>
-      <c r="F22" s="15"/>
+      <c r="D22" s="14"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:10" ht="15">
-      <c r="D23" s="15"/>
-      <c r="F23" s="16"/>
+      <c r="D23" s="14"/>
+      <c r="F23" s="15"/>
     </row>
     <row r="24" spans="2:10" ht="15">
-      <c r="F24" s="16"/>
+      <c r="F24" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2603,35 +2603,35 @@
   <sheetData>
     <row r="2" spans="2:4" ht="15.6" customHeight="1"/>
     <row r="3" spans="2:4" ht="30" customHeight="1">
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="22" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="46.8" customHeight="1">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="35">
         <v>44460</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="48" customHeight="1">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="39">
+      <c r="C5" s="36">
         <v>44464</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Review and change of all documentation
Review and change of all documentation
</commit_message>
<xml_diff>
--- a/04-TEST/PRUEBAS UNITARIAS/PLANTILLA_PRUEBAS_DE_SOFTWARE/Plantilla_Pruebas_de_Software_S.O.E.xlsx
+++ b/04-TEST/PRUEBAS UNITARIAS/PLANTILLA_PRUEBAS_DE_SOFTWARE/Plantilla_Pruebas_de_Software_S.O.E.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c7f5dae58cac8d6/Documentos/SOE/04-TEST/PRUEBAS UNITARIAS/PLANTILLA_PRUEBAS_DE_SOFTWARE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{D28DF50D-15A6-46AF-9D54-C878F891D79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6351C99-1476-4283-8324-26225D8B0E14}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{D28DF50D-15A6-46AF-9D54-C878F891D79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7022C31-B0B7-4D29-924A-AE40188CB5E9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Inicio Sesión" sheetId="1" r:id="rId1"/>
-    <sheet name="Registro usuario" sheetId="2" r:id="rId2"/>
+    <sheet name="Registro usuario" sheetId="2" r:id="rId1"/>
+    <sheet name="Inicio Sesión" sheetId="1" r:id="rId2"/>
     <sheet name="Validar Usuario" sheetId="3" r:id="rId3"/>
     <sheet name="Consultar Usuario" sheetId="4" r:id="rId4"/>
     <sheet name="Interfaz Amigable" sheetId="5" r:id="rId5"/>
@@ -724,13 +724,13 @@
     <xf numFmtId="14" fontId="13" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -749,6 +749,49 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>299258</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>52818</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6331527" cy="3383107"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="image1.png" title="Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{646B844B-4DD8-46AF-97AF-F9A0B372E73C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11756967" y="828673"/>
+          <a:ext cx="6331527" cy="3383107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -778,49 +821,6 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11693237" y="787110"/>
-          <a:ext cx="6331527" cy="3383107"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>299258</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>52818</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="6331527" cy="3383107"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="image1.png" title="Imagen">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{646B844B-4DD8-46AF-97AF-F9A0B372E73C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11756967" y="828673"/>
           <a:ext cx="6331527" cy="3383107"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1241,14 +1241,284 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="B2:J24"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="2" max="2" width="28.5546875" customWidth="1"/>
+    <col min="3" max="3" width="41.5546875" customWidth="1"/>
+    <col min="4" max="4" width="61.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="40.77734375" customWidth="1"/>
+    <col min="7" max="8" width="41.109375" customWidth="1"/>
+    <col min="9" max="9" width="21.33203125" customWidth="1"/>
+    <col min="10" max="10" width="21.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" ht="15">
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:10" ht="15">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="2:10" ht="15">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="2:10" ht="15.6">
+      <c r="B5" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="39"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="2:10" ht="27.75" customHeight="1">
+      <c r="B6" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="2:10" ht="60">
+      <c r="B7" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="2:10" ht="28.5" customHeight="1">
+      <c r="B8" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="6">
+        <v>44460</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="2:10" ht="26.25" customHeight="1">
+      <c r="B9" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="6">
+        <v>44464</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="28.5" customHeight="1">
+      <c r="B10" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+    </row>
+    <row r="11" spans="2:10" ht="30" customHeight="1">
+      <c r="B11" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="42.6" customHeight="1">
+      <c r="B12" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="61.2" customHeight="1"/>
+    <row r="16" spans="2:10" ht="82.8" customHeight="1">
+      <c r="B16" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="100.2" customHeight="1">
+      <c r="B17" s="29">
+        <v>5</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" s="11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="100.2" customHeight="1">
+      <c r="B18" s="29">
+        <v>6</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18" s="11">
+        <v>0.50347222222222221</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="100.8" customHeight="1">
+      <c r="B19" s="29">
+        <v>7</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="11">
+        <v>0.50347222222222221</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="100.8" customHeight="1">
+      <c r="B20" s="29">
+        <v>8</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="11">
+        <v>0.50347222222222221</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="13.2">
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+    </row>
+    <row r="22" spans="2:10" ht="15">
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+    </row>
+    <row r="23" spans="2:10" ht="15">
+      <c r="D23" s="14"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="2:10" ht="15">
+      <c r="E24" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="B2:J24"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1274,10 +1544,10 @@
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="2:10" ht="15.6">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="38"/>
+      <c r="C5" s="39"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="2:10" ht="27.75" customHeight="1">
@@ -1359,7 +1629,7 @@
       <c r="G16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="39" t="s">
+      <c r="H16" s="37" t="s">
         <v>17</v>
       </c>
       <c r="I16" s="8" t="s">
@@ -1499,276 +1769,6 @@
     </row>
     <row r="24" spans="2:10" ht="15">
       <c r="F24" s="15"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B5:C5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="B2:J24"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
-  <cols>
-    <col min="2" max="2" width="28.5546875" customWidth="1"/>
-    <col min="3" max="3" width="41.5546875" customWidth="1"/>
-    <col min="4" max="4" width="61.44140625" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="40.77734375" customWidth="1"/>
-    <col min="7" max="8" width="41.109375" customWidth="1"/>
-    <col min="9" max="9" width="21.33203125" customWidth="1"/>
-    <col min="10" max="10" width="21.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:10" ht="15">
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:10" ht="15">
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="2:10" ht="15">
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="2:10" ht="15.6">
-      <c r="B5" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="2:10" ht="27.75" customHeight="1">
-      <c r="B6" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="2:10" ht="60">
-      <c r="B7" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="2:10" ht="28.5" customHeight="1">
-      <c r="B8" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="6">
-        <v>44460</v>
-      </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="2:10" ht="26.25" customHeight="1">
-      <c r="B9" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="6">
-        <v>44464</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" ht="28.5" customHeight="1">
-      <c r="B10" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-    </row>
-    <row r="11" spans="2:10" ht="30" customHeight="1">
-      <c r="B11" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="27" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" ht="42.6" customHeight="1">
-      <c r="B12" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" ht="61.2" customHeight="1"/>
-    <row r="16" spans="2:10" ht="82.8" customHeight="1">
-      <c r="B16" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="C16" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" ht="100.2" customHeight="1">
-      <c r="B17" s="29">
-        <v>5</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" s="11">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="100.2" customHeight="1">
-      <c r="B18" s="29">
-        <v>6</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J18" s="11">
-        <v>0.50347222222222221</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="100.8" customHeight="1">
-      <c r="B19" s="29">
-        <v>7</v>
-      </c>
-      <c r="C19" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H19" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="I19" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J19" s="11">
-        <v>0.50347222222222221</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" ht="100.8" customHeight="1">
-      <c r="B20" s="29">
-        <v>8</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J20" s="11">
-        <v>0.50347222222222221</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" ht="13.2">
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-    </row>
-    <row r="22" spans="2:10" ht="15">
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-    </row>
-    <row r="23" spans="2:10" ht="15">
-      <c r="D23" s="14"/>
-      <c r="E23" s="15"/>
-    </row>
-    <row r="24" spans="2:10" ht="15">
-      <c r="E24" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1786,8 +1786,8 @@
   </sheetPr>
   <dimension ref="B2:J24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1813,10 +1813,10 @@
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="38"/>
+      <c r="C5" s="39"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="2:10" ht="27.75" customHeight="1">
@@ -2082,10 +2082,10 @@
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="38"/>
+      <c r="C5" s="39"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="2:10" ht="27.75" customHeight="1">
@@ -2325,7 +2325,7 @@
   <dimension ref="B2:J24"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2351,10 +2351,10 @@
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="2:10" ht="26.4" customHeight="1">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="38"/>
+      <c r="C5" s="39"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="2:10" ht="27.75" customHeight="1">

</xml_diff>